<commit_message>
added old PCB stuff from Charles
</commit_message>
<xml_diff>
--- a/New PCB Test Plan.xlsx
+++ b/New PCB Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\UROP_S2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF56219-EE08-4B1B-8F8B-122AAC5CAC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283CB8E7-CD61-4FF2-A850-0BAFDE6AB757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Test Name</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Vgs voltages are what we expect them to be, current readings from transimpedance amplifer are accurate, power rails are stable.</t>
   </si>
   <si>
-    <t>Plug the three main PCBs together. Hook up power supply set to 3.7V to VBATT and turn on main power switch. Measure the power rails.</t>
-  </si>
-  <si>
     <t>LiPo</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Connect USB-C to PCB to charge the LiPo.</t>
   </si>
   <si>
-    <t>Voltage rails should turn off. Charge LED should turn on (orange). Voltage of battery slowly increases. When charging is done, charge LED turns white.</t>
-  </si>
-  <si>
     <t>Gate Voltage Power Rails</t>
   </si>
   <si>
@@ -201,8 +195,23 @@
     <t>ESP32 serial reports correct thermistor readings.</t>
   </si>
   <si>
+    <t>Before the heater is turned on, the output should be 0V. When heater is turned on, the output is about 7V.  Heater ON LED turns on.</t>
+  </si>
+  <si>
+    <t>Humidity Sensor</t>
+  </si>
+  <si>
+    <t>Connect BME680 to main PCB assembly. Run BME680_test.</t>
+  </si>
+  <si>
+    <t>Serial reports reasonable temp readings and humidity readings. When you breathe on the sensor, the humidity and temperature should rise.</t>
+  </si>
+  <si>
+    <t>Plug the three main PCBs together. Hook up power supply set to 3.7V to VBATT and turn on main power switch. Measure the power rails. Then sweep power supply input from 3V to 4.2V.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1V, 2V, and 3V3 rails all are close to their expected value. +-11V rails should be </t>
+      <t xml:space="preserve">1V, 2V, and 3V3 rails all are close to their expected value. VIN should be around 3.3V due to reverse diode. +-11V rails should be </t>
     </r>
     <r>
       <rPr>
@@ -221,27 +230,36 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>. Current consumption looks ok (&lt;100 mA). ON LED turns on.</t>
+      <t>. Current consumption looks ok (&lt;100 mA). LOWBATT signal should go low once input is below 3.3V.</t>
     </r>
   </si>
   <si>
-    <t>Before the heater is turned on, the output should be 0V. When heater is turned on, the output is about 7V.  Heater ON LED turns on.</t>
-  </si>
-  <si>
-    <t>Humidity Sensor</t>
-  </si>
-  <si>
-    <t>Connect BME680 to main PCB assembly. Run BME680_test.</t>
-  </si>
-  <si>
-    <t>Serial reports reasonable temp readings and humidity readings. When you breathe on the sensor, the humidity and temperature should rise.</t>
+    <t>Voltage rails should turn off. Max charging current should be around 0.8A. Charge LED should turn on (orange). Voltage of battery slowly increases. When charging is done, charge LED turns white.</t>
+  </si>
+  <si>
+    <t>Important Things to Remember</t>
+  </si>
+  <si>
+    <t>Plug in ESP32 properly (USB side is facing the side labeled "FRONT"</t>
+  </si>
+  <si>
+    <t>Do not turn the ON switch on and plug into the ESP32 USB at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current draw is 13 mA at 3.7V. +11V rail is at around 3V, -11v rail is at 0.5V. !V rail is at 0.993V, 2V rail is at 2.004V. LOWBATT triggers at 3.15V. </t>
+  </si>
+  <si>
+    <t>Bottom PCB has to be disconnected for this test.</t>
+  </si>
+  <si>
+    <t>(positive offset means measured is higher than expected) Channel 0: +20mV, Channel 1: -5mV, Channel 2: +20 mV, Channel 3: no offset,  Channel 4: +10 mV, Channel 5: no offset, Channel 6: -5 mV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +280,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -318,6 +350,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,297 +647,259 @@
     <col min="3" max="3" width="41.5546875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="7" spans="1:6" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="88.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
-    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
@@ -919,30 +917,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+    <row r="27" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+    <row r="28" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="2"/>
     </row>
@@ -954,16 +964,32 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="2"/>
     </row>
@@ -990,7 +1016,7 @@
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="4"/>
       <c r="E35" s="2"/>
@@ -1002,6 +1028,41 @@
       <c r="D36" s="4"/>
       <c r="E36" s="2"/>
     </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>